<commit_message>
tested several excel configurations
</commit_message>
<xml_diff>
--- a/dist/analysis/log.xlsx
+++ b/dist/analysis/log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
   <si>
     <t>Excel</t>
   </si>
@@ -227,6 +227,156 @@
   </si>
   <si>
     <t>48</t>
+  </si>
+  <si>
+    <t>.\1.xlsx</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>26000</t>
+  </si>
+  <si>
+    <t>25991</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>504</t>
+  </si>
+  <si>
+    <t>75000</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1668</t>
+  </si>
+  <si>
+    <t>8340</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>24000</t>
+  </si>
+  <si>
+    <t>3984</t>
+  </si>
+  <si>
+    <t>3336</t>
+  </si>
+  <si>
+    <t>16680</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>36000</t>
+  </si>
+  <si>
+    <t>5976</t>
+  </si>
+  <si>
+    <t>5004</t>
+  </si>
+  <si>
+    <t>25020</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>241</t>
   </si>
 </sst>
 </file>
@@ -588,9 +738,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1718,6 +1868,1222 @@
         <v>63</v>
       </c>
     </row>
+    <row r="30" spans="1:15">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J31" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" t="s">
+        <v>36</v>
+      </c>
+      <c r="J33" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" t="s">
+        <v>36</v>
+      </c>
+      <c r="J34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" t="s">
+        <v>36</v>
+      </c>
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J36" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" t="s">
+        <v>36</v>
+      </c>
+      <c r="J37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" t="s">
+        <v>36</v>
+      </c>
+      <c r="L37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I39" t="s">
+        <v>36</v>
+      </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J40" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" t="s">
+        <v>36</v>
+      </c>
+      <c r="K41" t="s">
+        <v>36</v>
+      </c>
+      <c r="L41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" t="s">
+        <v>36</v>
+      </c>
+      <c r="L42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" t="s">
+        <v>36</v>
+      </c>
+      <c r="J43" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" t="s">
+        <v>36</v>
+      </c>
+      <c r="L43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44" t="s">
+        <v>86</v>
+      </c>
+      <c r="H44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" t="s">
+        <v>36</v>
+      </c>
+      <c r="J44" t="s">
+        <v>36</v>
+      </c>
+      <c r="K44" t="s">
+        <v>36</v>
+      </c>
+      <c r="L44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45" t="s">
+        <v>87</v>
+      </c>
+      <c r="I45" t="s">
+        <v>36</v>
+      </c>
+      <c r="J45" t="s">
+        <v>36</v>
+      </c>
+      <c r="K45" t="s">
+        <v>36</v>
+      </c>
+      <c r="L45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" t="s">
+        <v>36</v>
+      </c>
+      <c r="G46" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" t="s">
+        <v>89</v>
+      </c>
+      <c r="I46" t="s">
+        <v>36</v>
+      </c>
+      <c r="J46" t="s">
+        <v>36</v>
+      </c>
+      <c r="K46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" t="s">
+        <v>96</v>
+      </c>
+      <c r="H47" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47" t="s">
+        <v>36</v>
+      </c>
+      <c r="J47" t="s">
+        <v>36</v>
+      </c>
+      <c r="K47" t="s">
+        <v>36</v>
+      </c>
+      <c r="L47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" t="s">
+        <v>36</v>
+      </c>
+      <c r="I48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" t="s">
+        <v>36</v>
+      </c>
+      <c r="K48" t="s">
+        <v>36</v>
+      </c>
+      <c r="L48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" t="s">
+        <v>36</v>
+      </c>
+      <c r="J49" t="s">
+        <v>36</v>
+      </c>
+      <c r="K49" t="s">
+        <v>36</v>
+      </c>
+      <c r="L49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" t="s">
+        <v>36</v>
+      </c>
+      <c r="H50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" t="s">
+        <v>36</v>
+      </c>
+      <c r="J50" t="s">
+        <v>36</v>
+      </c>
+      <c r="K50" t="s">
+        <v>36</v>
+      </c>
+      <c r="L50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" t="s">
+        <v>36</v>
+      </c>
+      <c r="I51" t="s">
+        <v>36</v>
+      </c>
+      <c r="J51" t="s">
+        <v>36</v>
+      </c>
+      <c r="K51" t="s">
+        <v>36</v>
+      </c>
+      <c r="L51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J52" t="s">
+        <v>36</v>
+      </c>
+      <c r="K52" t="s">
+        <v>36</v>
+      </c>
+      <c r="L52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" t="s">
+        <v>36</v>
+      </c>
+      <c r="G53" t="s">
+        <v>87</v>
+      </c>
+      <c r="H53" t="s">
+        <v>87</v>
+      </c>
+      <c r="I53" t="s">
+        <v>36</v>
+      </c>
+      <c r="J53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K53" t="s">
+        <v>36</v>
+      </c>
+      <c r="L53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" t="s">
+        <v>101</v>
+      </c>
+      <c r="F54" t="s">
+        <v>102</v>
+      </c>
+      <c r="G54" t="s">
+        <v>103</v>
+      </c>
+      <c r="H54" t="s">
+        <v>103</v>
+      </c>
+      <c r="I54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J54" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" t="s">
+        <v>16</v>
+      </c>
+      <c r="L54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" t="s">
+        <v>107</v>
+      </c>
+      <c r="F55" t="s">
+        <v>108</v>
+      </c>
+      <c r="G55" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" t="s">
+        <v>103</v>
+      </c>
+      <c r="I55" t="s">
+        <v>36</v>
+      </c>
+      <c r="J55" t="s">
+        <v>104</v>
+      </c>
+      <c r="K55" t="s">
+        <v>16</v>
+      </c>
+      <c r="L55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>106</v>
+      </c>
+      <c r="E56" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" t="s">
+        <v>108</v>
+      </c>
+      <c r="G56" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" t="s">
+        <v>103</v>
+      </c>
+      <c r="I56" t="s">
+        <v>36</v>
+      </c>
+      <c r="J56" t="s">
+        <v>104</v>
+      </c>
+      <c r="K56" t="s">
+        <v>16</v>
+      </c>
+      <c r="L56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>106</v>
+      </c>
+      <c r="E57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" t="s">
+        <v>108</v>
+      </c>
+      <c r="G57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H57" t="s">
+        <v>103</v>
+      </c>
+      <c r="I57" t="s">
+        <v>36</v>
+      </c>
+      <c r="J57" t="s">
+        <v>104</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" t="s">
+        <v>115</v>
+      </c>
+      <c r="G58" t="s">
+        <v>116</v>
+      </c>
+      <c r="H58" t="s">
+        <v>103</v>
+      </c>
+      <c r="I58" t="s">
+        <v>36</v>
+      </c>
+      <c r="J58" t="s">
+        <v>104</v>
+      </c>
+      <c r="K58" t="s">
+        <v>16</v>
+      </c>
+      <c r="L58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" t="s">
+        <v>114</v>
+      </c>
+      <c r="F59" t="s">
+        <v>115</v>
+      </c>
+      <c r="G59" t="s">
+        <v>116</v>
+      </c>
+      <c r="H59" t="s">
+        <v>103</v>
+      </c>
+      <c r="I59" t="s">
+        <v>36</v>
+      </c>
+      <c r="J59" t="s">
+        <v>104</v>
+      </c>
+      <c r="K59" t="s">
+        <v>16</v>
+      </c>
+      <c r="L59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" t="s">
+        <v>115</v>
+      </c>
+      <c r="G60" t="s">
+        <v>116</v>
+      </c>
+      <c r="H60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I60" t="s">
+        <v>36</v>
+      </c>
+      <c r="J60" t="s">
+        <v>104</v>
+      </c>
+      <c r="K60" t="s">
+        <v>16</v>
+      </c>
+      <c r="L60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61" t="s">
+        <v>114</v>
+      </c>
+      <c r="F61" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" t="s">
+        <v>116</v>
+      </c>
+      <c r="H61" t="s">
+        <v>103</v>
+      </c>
+      <c r="I61" t="s">
+        <v>36</v>
+      </c>
+      <c r="J61" t="s">
+        <v>104</v>
+      </c>
+      <c r="K61" t="s">
+        <v>16</v>
+      </c>
+      <c r="L61" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.787401575" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.787401575"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
commit after longer use of app
</commit_message>
<xml_diff>
--- a/dist/analysis/log.xlsx
+++ b/dist/analysis/log.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
   <si>
     <t>Excel</t>
   </si>
@@ -377,6 +378,90 @@
   </si>
   <si>
     <t>241</t>
+  </si>
+  <si>
+    <t>.\180720 FBP tool v0.17.xlsx</t>
+  </si>
+  <si>
+    <t>2660</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>6106742</t>
+  </si>
+  <si>
+    <t>5950658</t>
+  </si>
+  <si>
+    <t>41568</t>
+  </si>
+  <si>
+    <t>60224</t>
+  </si>
+  <si>
+    <t>8392</t>
+  </si>
+  <si>
+    <t>54292</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>1.31</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>.\test.xlsx</t>
+  </si>
+  <si>
+    <t>741</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>314</t>
+  </si>
+  <si>
+    <t>.\BC17.xlsx</t>
+  </si>
+  <si>
+    <t>2658</t>
+  </si>
+  <si>
+    <t>6107246</t>
+  </si>
+  <si>
+    <t>5951045</t>
+  </si>
+  <si>
+    <t>41601</t>
+  </si>
+  <si>
+    <t>60244</t>
+  </si>
+  <si>
+    <t>9990</t>
+  </si>
+  <si>
+    <t>54356</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>change (%)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -429,6 +514,18 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Standard" xfId="0"/>
@@ -738,10 +835,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -3084,8 +3181,413 @@
         <v>117</v>
       </c>
     </row>
+    <row r="62" spans="1:15">
+      <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" t="s">
+        <v>124</v>
+      </c>
+      <c r="E62" t="s">
+        <v>125</v>
+      </c>
+      <c r="F62" t="s">
+        <v>126</v>
+      </c>
+      <c r="G62" t="s">
+        <v>127</v>
+      </c>
+      <c r="H62" t="s">
+        <v>128</v>
+      </c>
+      <c r="I62" t="s">
+        <v>129</v>
+      </c>
+      <c r="J62" t="s">
+        <v>130</v>
+      </c>
+      <c r="K62" t="s">
+        <v>131</v>
+      </c>
+      <c r="L62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" t="s">
+        <v>135</v>
+      </c>
+      <c r="F63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G63" t="s">
+        <v>36</v>
+      </c>
+      <c r="H63" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" t="s">
+        <v>36</v>
+      </c>
+      <c r="J63" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" t="s">
+        <v>16</v>
+      </c>
+      <c r="L63" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" t="s">
+        <v>140</v>
+      </c>
+      <c r="F64" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" t="s">
+        <v>142</v>
+      </c>
+      <c r="H64" t="s">
+        <v>143</v>
+      </c>
+      <c r="I64" t="s">
+        <v>144</v>
+      </c>
+      <c r="J64" t="s">
+        <v>130</v>
+      </c>
+      <c r="K64" t="s">
+        <v>131</v>
+      </c>
+      <c r="L64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>139</v>
+      </c>
+      <c r="E65" t="s">
+        <v>140</v>
+      </c>
+      <c r="F65" t="s">
+        <v>141</v>
+      </c>
+      <c r="G65" t="s">
+        <v>142</v>
+      </c>
+      <c r="H65" t="s">
+        <v>143</v>
+      </c>
+      <c r="I65" t="s">
+        <v>144</v>
+      </c>
+      <c r="J65" t="s">
+        <v>130</v>
+      </c>
+      <c r="K65" t="s">
+        <v>131</v>
+      </c>
+      <c r="L65" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.787401575" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.787401575"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="27.85546875"/>
+    <col customWidth="1" max="4" min="2" width="12.28515625"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="7" spans="1:15">
+      <c r="A2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="8" t="n"/>
+    </row>
+    <row customFormat="1" r="3" s="7" spans="1:15">
+      <c r="A3" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="8" t="n">
+        <v>712</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>4350802</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>4331121</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>5142</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>7758</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>7233</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>6781</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N3" s="8" t="n"/>
+      <c r="O3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>712</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="4">
+        <f>C7/B7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>5142</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="4">
+        <f>C8/B8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>7758</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="4">
+        <f>C9/B9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>7233</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="4">
+        <f>C10/B10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>6781</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="4">
+        <f>C11/B11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="D12" s="4">
+        <f>C12/B12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="9" t="n"/>
+      <c r="C13" s="9" t="n"/>
+      <c r="D13" s="4" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.787401575" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.787401575"/>
+</worksheet>
 </file>
</xml_diff>